<commit_message>
product /service/book import done
</commit_message>
<xml_diff>
--- a/public/export/book-import-sample-file-service-provider.xlsx
+++ b/public/export/book-import-sample-file-service-provider.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\www\student-store-api\public\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74602E3E-968E-48B8-B5F8-647332152E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD752EF-FC14-4066-B37E-FA438E8AA471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DE495C39-57E1-42E3-B52A-6F62DE5635B2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>type</t>
   </si>
@@ -43,15 +43,6 @@
     <t>is_on_offer</t>
   </si>
   <si>
-    <t>brand_name</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>gtin_number</t>
-  </si>
-  <si>
     <t>discount_type</t>
   </si>
   <si>
@@ -61,9 +52,6 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>product_description</t>
-  </si>
-  <si>
     <t>delivery_type</t>
   </si>
   <si>
@@ -73,21 +61,6 @@
     <t>images</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
-  <si>
-    <t>Apple Smart Watch 2.0</t>
-  </si>
-  <si>
-    <t>sku154318554</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -103,25 +76,76 @@
     <t>deliver_to_location</t>
   </si>
   <si>
-    <t>Apple Smart Watch 3.0</t>
-  </si>
-  <si>
-    <t>sku154310124</t>
-  </si>
-  <si>
-    <t>percentage</t>
-  </si>
-  <si>
     <t>Apple 2.0 Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy</t>
   </si>
   <si>
-    <t>Apple 3.0 Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy</t>
-  </si>
-  <si>
-    <t>pickup_from_location</t>
-  </si>
-  <si>
     <t>actual_price</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>One time</t>
+  </si>
+  <si>
+    <t>sku15431655</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>sell_type</t>
+  </si>
+  <si>
+    <t>published_year</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>no_of_pages</t>
+  </si>
+  <si>
+    <t>suitable_age</t>
+  </si>
+  <si>
+    <t>dimension_length</t>
+  </si>
+  <si>
+    <t>dimension_width</t>
+  </si>
+  <si>
+    <t>dimension_height</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>for_sale</t>
+  </si>
+  <si>
+    <t>Jhon Doe</t>
+  </si>
+  <si>
+    <t>Jhony Cxom</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>18 years and above</t>
+  </si>
+  <si>
+    <t>isbn_number</t>
+  </si>
+  <si>
+    <t>book_description</t>
+  </si>
+  <si>
+    <t>book_name</t>
+  </si>
+  <si>
+    <t>languages</t>
   </si>
 </sst>
 </file>
@@ -473,169 +497,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08470AB-C17C-45CE-BA84-CEA747715504}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="111.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="111.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>484333451</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>2011</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2">
+        <v>100</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="T2">
+        <v>15</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+      <c r="V2">
+        <v>250</v>
+      </c>
+      <c r="W2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="X2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>4845481451</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2">
-        <v>1500</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3">
-        <v>4845481400</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3">
-        <v>1800</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{E1BC0B34-2A86-41B9-AAAF-A0DEFE22D17F}">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{E1BC0B34-2A86-41B9-AAAF-A0DEFE22D17F}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{1D38C07A-DA75-4D62-9C59-14390CEEB4E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{1D38C07A-DA75-4D62-9C59-14390CEEB4E8}">
       <formula1>"fixed_amount, percentage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3" xr:uid="{BB274958-8C16-4C20-9DA1-738E90234607}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{BB274958-8C16-4C20-9DA1-738E90234607}">
       <formula1>"deliver_to_location,pickup_from_location"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{AADBF204-4524-4C0D-99BA-873D67E8F405}">
+      <formula1>"free,for_sale"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{00122B88-6AED-4A12-BBF9-13E3CF6310D6}">
+      <formula1>1900</formula1>
+      <formula2>2100</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2 S2 T1 U1 T2 U2 V2" xr:uid="{D27C4032-13A6-4D38-871A-AEED393D78CC}">
+      <formula1>1</formula1>
+      <formula2>5000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{36095326-2D0B-407D-AF64-11449BF5550E}">
+      <formula1>"5 to 9 years,9 to 13 years,13 to 18 years,18 years and above"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1" xr:uid="{18A6EBB2-23AB-4E95-9DDD-E6AF7EE1A740}">
+      <formula1>0.1</formula1>
+      <formula2>5000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel file added validation
</commit_message>
<xml_diff>
--- a/public/export/book-import-sample-file-service-provider.xlsx
+++ b/public/export/book-import-sample-file-service-provider.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\www\student-store-api\public\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CD306F-29AA-4BD1-B97E-A8793CF4458A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA7B35-3BD8-4EC8-9141-35AC608F05DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1481,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1643,7 +1643,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"deliver_to_location,pickup_from_location"</formula1>
     </dataValidation>
@@ -1677,6 +1677,9 @@
       <formula1>1500</formula1>
       <formula2>2200</formula2>
     </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{0B657622-FFEB-49F5-902E-18562E221D89}">
+      <formula1>"book"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
free sell type import data fixed
</commit_message>
<xml_diff>
--- a/public/export/book-import-sample-file-service-provider.xlsx
+++ b/public/export/book-import-sample-file-service-provider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\www\student-store-api\public\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA7B35-3BD8-4EC8-9141-35AC608F05DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA8250C-0AE0-444C-8FEA-A4509EA76D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1481,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="I2" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,9 +1646,6 @@
   <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"deliver_to_location,pickup_from_location"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"free,for_sale"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>1900</formula1>
@@ -1680,6 +1677,9 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{0B657622-FFEB-49F5-902E-18562E221D89}">
       <formula1>"book"</formula1>
     </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{B07E712A-E268-4EED-9820-C356AEC9C345}">
+      <formula1>"free,for_sale"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>